<commit_message>
Updated with status for user to see when selecting a player.
</commit_message>
<xml_diff>
--- a/Forms/Playoff Fantasy Football - 2023-2024 Signup Roster.xlsx
+++ b/Forms/Playoff Fantasy Football - 2023-2024 Signup Roster.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamx\Local Documents\Playoff Fantasy Football\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamx\Local Documents\Playoff Fantasy Football\NFL_Playoff_Fantasy_HelpeR\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21415D9E-F2E9-4137-819E-EBEDF0BBB308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ekTP8VEApalA6Qi76a6NTLUDxaPZh5gMsCN1Ckw6kaY4nntAvsBEy0kU3g966S15g3s3iiB2xb+31QJjVb0nKg==" workbookSaltValue="In/N1KZb9cSlqLEHCozWXg==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8F7AB2-6FB2-47DB-A90A-108E325266B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="13680" tabRatio="760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10545" yWindow="-21720" windowWidth="51840" windowHeight="21120" tabRatio="760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Roster" sheetId="33" r:id="rId1"/>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10177" uniqueCount="2365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10179" uniqueCount="2367">
   <si>
     <t>QB</t>
   </si>
@@ -7163,6 +7162,12 @@
   </si>
   <si>
     <t>Complete all cells in blue.</t>
+  </si>
+  <si>
+    <t>Player Status</t>
+  </si>
+  <si>
+    <t>Player Status Short Description</t>
   </si>
 </sst>
 </file>
@@ -7330,7 +7335,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -7350,6 +7355,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7366,11 +7372,17 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7384,14 +7396,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8748,18 +8760,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB9BE899-55DA-4AD4-94FD-5C3DAAC6B45B}" name="Table1" displayName="Table1" ref="B6:M20" totalsRowShown="0">
-  <tableColumns count="12">
-    <tableColumn id="5" xr3:uid="{4BCFD665-B3C4-476C-B080-DFEC67DF0AA0}" name="Fantasy Owner" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB9BE899-55DA-4AD4-94FD-5C3DAAC6B45B}" name="Table1" displayName="Table1" ref="B6:O20" totalsRowShown="0">
+  <tableColumns count="14">
+    <tableColumn id="5" xr3:uid="{4BCFD665-B3C4-476C-B080-DFEC67DF0AA0}" name="Fantasy Owner" dataDxfId="13">
       <calculatedColumnFormula>IF($G$2="","",$G$2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A7D56874-89BF-4E4F-A281-CA22E20BF820}" name="Fantasy Owner Email" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{A7D56874-89BF-4E4F-A281-CA22E20BF820}" name="Fantasy Owner Email" dataDxfId="12">
       <calculatedColumnFormula>IF($G$3="","",$G$3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C75B8E0E-F513-41D6-B787-B8B73B348F93}" name="Fantasy Team Name" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{C75B8E0E-F513-41D6-B787-B8B73B348F93}" name="Fantasy Team Name" dataDxfId="11">
       <calculatedColumnFormula>IF($G$4="","",$G$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{7D54152C-4AC0-4D3B-9FFD-1C31EC010A79}" name="Automation Mapping" dataDxfId="8">
+    <tableColumn id="14" xr3:uid="{7D54152C-4AC0-4D3B-9FFD-1C31EC010A79}" name="Automation Mapping" dataDxfId="10">
       <calculatedColumnFormula array="1">IF(Table1[[#This Row],[Selection]]="","",
 IF(Table1[[#This Row],[Position Type]]="Defense / Special Teams",Table1[[#This Row],[Team Abbr.]],
 _xlfn._xlws.FILTER(INDIRECT("tbl"&amp;Table1[[#This Row],[Position Group]]&amp;"[gsis_id_"&amp;Table1[[#This Row],[Position Group]]&amp;"]"),INDIRECT("tbl"&amp;Table1[[#This Row],[Position Group]]&amp;"[selector_id_"&amp;Table1[[#This Row],[Position Group]]&amp;"]")=Table1[[#This Row],[Selection]])))</calculatedColumnFormula>
@@ -8768,15 +8780,31 @@
     <tableColumn id="4" xr3:uid="{1F320687-788D-46D7-86EB-AD2965521E00}" name="Position Type"/>
     <tableColumn id="2" xr3:uid="{D393BDB1-6485-419D-8243-1EE88DDD2700}" name="Position Code"/>
     <tableColumn id="1" xr3:uid="{B0BEDE34-C385-49DE-BD3C-CC76AF38DD1C}" name="Position Group"/>
-    <tableColumn id="7" xr3:uid="{606F1564-FF41-4770-B3CD-2A010E0B9627}" name="Selection" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{0ACCB11F-2DE0-48FA-8482-81CB381DC9F6}" name="Team Abbr." dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{606F1564-FF41-4770-B3CD-2A010E0B9627}" name="Selection" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{0ACCB11F-2DE0-48FA-8482-81CB381DC9F6}" name="Team Abbr." dataDxfId="8">
       <calculatedColumnFormula array="1">IF(Table1[[#This Row],[Selection]]="","",_xlfn._xlws.FILTER(INDIRECT("tbl"&amp;Table1[[#This Row],[Position Group]]&amp;"[team_abbr_"&amp;Table1[[#This Row],[Position Group]]&amp;"]"),INDIRECT("tbl"&amp;Table1[[#This Row],[Position Group]]&amp;"[selector_id_"&amp;Table1[[#This Row],[Position Group]]&amp;"]")=Table1[[#This Row],[Selection]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B8BCBCC7-9558-45B9-BBE4-85EF9ACDCD31}" name="Check 1 - Selection is Unique" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{B8BCBCC7-9558-45B9-BBE4-85EF9ACDCD31}" name="Check 1 - Selection is Unique" dataDxfId="7">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Selection],Table1[[#This Row],[Selection]])=1,TRUE,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{58E11982-4558-4D0F-B1B7-2457EE65E044}" name="Check 2 - Team is Unique" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{58E11982-4558-4D0F-B1B7-2457EE65E044}" name="Check 2 - Team is Unique" dataDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7F94DB03-1380-41DE-967F-8248509C730F}" name="Player Status" dataDxfId="1">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{F5B99BB8-38D7-4DF4-AF63-99F39572DD6E}" name="Player Status Short Description" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9228,19 +9256,19 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:M754"/>
+  <dimension ref="B1:O754"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="19.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="19" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="20.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
@@ -9248,32 +9276,34 @@
     <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F1" s="10" t="s">
         <v>2364</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F2" s="3" t="s">
         <v>2362</v>
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="F3" s="5" t="s">
         <v>2363</v>
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F4" s="7" t="s">
         <v>1513</v>
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1514</v>
       </c>
@@ -9310,8 +9340,14 @@
       <c r="M6" t="s">
         <v>2292</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>2365</v>
+      </c>
+      <c r="O6" t="s">
+        <v>2366</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f t="shared" ref="B7:B20" si="0">IF($G$2="","",$G$2)</f>
         <v/>
@@ -9355,8 +9391,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N7" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O7" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9400,8 +9454,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N8" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O8" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9445,8 +9517,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N9" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O9" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9490,8 +9580,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N10" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O10" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9535,8 +9643,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N11" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O11" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9580,8 +9706,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N12" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O12" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9625,8 +9769,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N13" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O13" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9670,8 +9832,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N14" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O14" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9715,8 +9895,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N15" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O15" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9760,8 +9958,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O16" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9805,8 +10021,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O17" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9851,8 +10085,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N18" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O18" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9897,8 +10149,26 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N19" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+      <c r="O19" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9942,6 +10212,24 @@
         <f>IF(Table1[[#This Row],[Selection]]="","",IF(COUNTIFS(Table1[Team Abbr.],Table1[[#This Row],[Team Abbr.]])=1,TRUE,FALSE))</f>
         <v/>
       </c>
+      <c r="N20" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_SPEC],""),"N/A"))))))</f>
+        <v>N/A</v>
+      </c>
+      <c r="O20" s="11" t="str">
+        <f>IF(Table1[[#This Row],[Position Group]]="QB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblQB[selector_id_QB],tblQB[status_short_description_QB],""),
+IF(Table1[[#This Row],[Position Group]]="RB",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblRB[selector_id_RB],tblRB[status_short_description_RB],""),
+IF(Table1[[#This Row],[Position Group]]="WR",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblWR[selector_id_WR],tblWR[status_short_description_WR],""),
+IF(Table1[[#This Row],[Position Group]]="TE",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblTE[selector_id_TE],tblTE[status_short_description_TE],""),
+IF(Table1[[#This Row],[Position Group]]="FLEX",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblFLEX[selector_id_FLEX],tblFLEX[status_short_description_FLEX],""),
+IF(Table1[[#This Row],[Position Group]]="SPEC",_xlfn.XLOOKUP(Table1[[#This Row],[Selection]],tblSPEC[selector_id_SPEC],tblSPEC[status_short_description_SPEC],""),"N/A"))))))</f>
+        <v>N/A</v>
+      </c>
     </row>
     <row r="35" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M35" s="1"/>
@@ -11354,25 +11642,24 @@
       <c r="M754" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="0l4yBy9M+Lm4Ke2sQVg01snZ4mIJo0ADbVBl3w0stSxhj5wIs6HGaCfKM9xHY/PJwNxaYkva7XShGX6I9OD6bA==" saltValue="tJLyx3WSdMQaQF2RRSCVbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="G2:G4">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>G2=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J20 L7:L20">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>NOT($L7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J20">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>J7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K20 M7:M20">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>NOT($M7)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J20">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>J7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11434,7 +11721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D7577B-66CF-4055-9A19-3079D73ECB97}">
   <dimension ref="B2:BC539"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="J312" sqref="J312"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -46393,7 +46682,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F2tf4VUxI2mOjmvApXUYgIC9j1u5t53e8K3FoGa8TY4oqqJT0d7hZiLw9NE39XylWDgJG+pFAMIUueLD7bAFQA==" saltValue="B3VIQ5eFupZYAqXPh3MUdQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="6">
     <tablePart r:id="rId1"/>
@@ -46411,7 +46699,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46785,7 +47073,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="g/I/bLflCB0B1B0Gi/zWyPjn3bhseYMOMK/cmaIfUcQHqFyVeOOaWt7mRdFIp/+UW7qKYHHGyl5T7UbVQznQgw==" saltValue="mF+bKQMDmAwIREL6ZpvLcA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>